<commit_message>
agregar cambios de estudios
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepGitHubJavier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEA0D08-535E-4000-A159-7B20ED2A9EFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F9D6B-A996-4578-8A12-0907A9DC96DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2185,11 +2185,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O427"/>
+  <dimension ref="A1:O432"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A404" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E426" sqref="E1:E426"/>
+      <pane ySplit="1" topLeftCell="A413" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E429" sqref="E429:E432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6700,7 +6700,7 @@
         <v>44190</v>
       </c>
       <c r="E388" s="4">
-        <f t="shared" ref="E388:E426" si="6">SUM(B388,C388,D388)</f>
+        <f t="shared" ref="E388:E432" si="6">SUM(B388,C388,D388)</f>
         <v>0</v>
       </c>
     </row>
@@ -7085,6 +7085,85 @@
     <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" s="1">
         <v>44229</v>
+      </c>
+      <c r="B427" s="3">
+        <v>4.6967592592592589E-2</v>
+      </c>
+      <c r="D427" s="3">
+        <v>5.2430555555555557E-2</v>
+      </c>
+      <c r="E427" s="4">
+        <f>SUM(B427,B431,D427)</f>
+        <v>0.14277777777777778</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A428" s="1">
+        <v>44230</v>
+      </c>
+      <c r="B428" s="3">
+        <v>4.6944444444444448E-2</v>
+      </c>
+      <c r="D428" s="3">
+        <v>3.7430555555555557E-2</v>
+      </c>
+      <c r="E428" s="4">
+        <f t="shared" si="6"/>
+        <v>8.4375000000000006E-2</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A429" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B429" s="3">
+        <v>5.0173611111111106E-2</v>
+      </c>
+      <c r="D429" s="3">
+        <v>4.3124999999999997E-2</v>
+      </c>
+      <c r="E429" s="4">
+        <f>SUM(B429,D431,D429)</f>
+        <v>0.1232523148148148</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A430" s="1">
+        <v>44232</v>
+      </c>
+      <c r="B430" s="3">
+        <v>5.3530092592592594E-2</v>
+      </c>
+      <c r="D430" s="3">
+        <v>4.6967592592592589E-2</v>
+      </c>
+      <c r="E430" s="4">
+        <f t="shared" ref="E430:E432" si="7">SUM(B430,D432,D430)</f>
+        <v>0.10049768518518518</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A431" s="1">
+        <v>44233</v>
+      </c>
+      <c r="B431" s="3">
+        <v>4.3379629629629629E-2</v>
+      </c>
+      <c r="D431" s="3">
+        <v>2.9953703703703705E-2</v>
+      </c>
+      <c r="E431" s="4">
+        <f t="shared" si="7"/>
+        <v>7.3333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A432" s="1">
+        <v>44234</v>
+      </c>
+      <c r="E432" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
horas de estudio y ki8loton
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E436" sqref="E436"/>
+      <selection pane="bottomLeft" activeCell="B443" sqref="B443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7262,27 +7262,39 @@
       <c r="B440" s="3">
         <v>4.9085648148148149E-2</v>
       </c>
+      <c r="D440" s="3">
+        <v>4.6817129629629632E-2</v>
+      </c>
       <c r="E440" s="4">
         <f t="shared" si="6"/>
-        <v>4.9085648148148149E-2</v>
+        <v>9.5902777777777781E-2</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>44243</v>
       </c>
+      <c r="B441" s="3">
+        <v>4.7442129629629626E-2</v>
+      </c>
+      <c r="D441" s="3">
+        <v>2.5289351851851851E-2</v>
+      </c>
       <c r="E441" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7.273148148148148E-2</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>44244</v>
       </c>
+      <c r="B442" s="3">
+        <v>3.3483796296296296E-2</v>
+      </c>
       <c r="E442" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.3483796296296296E-2</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
las horas de estudio del 19 de feb 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D444" sqref="D444"/>
+      <selection pane="bottomLeft" activeCell="D445" sqref="D445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7319,9 +7319,15 @@
       <c r="A444" s="1">
         <v>44246</v>
       </c>
+      <c r="B444" s="3">
+        <v>4.1701388888888885E-2</v>
+      </c>
+      <c r="D444" s="3">
+        <v>4.2164351851851856E-2</v>
+      </c>
       <c r="E444" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8.3865740740740741E-2</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de lunes 22 de feb del 2020
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2184,11 +2184,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O445"/>
+  <dimension ref="A1:O455"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D445" sqref="D445"/>
+      <selection pane="bottomLeft" activeCell="D448" sqref="D448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6699,7 +6699,7 @@
         <v>44190</v>
       </c>
       <c r="E388" s="4">
-        <f t="shared" ref="E388:E445" si="6">SUM(B388,C388,D388)</f>
+        <f t="shared" ref="E388:E451" si="6">SUM(B388,C388,D388)</f>
         <v>0</v>
       </c>
     </row>
@@ -7338,6 +7338,90 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A446" s="1">
+        <v>44248</v>
+      </c>
+      <c r="E446" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A447" s="1">
+        <v>44249</v>
+      </c>
+      <c r="B447" s="3">
+        <v>4.9236111111111112E-2</v>
+      </c>
+      <c r="D447" s="3">
+        <v>4.731481481481481E-2</v>
+      </c>
+      <c r="E447" s="4">
+        <f t="shared" si="6"/>
+        <v>9.6550925925925929E-2</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A448" s="1">
+        <v>44250</v>
+      </c>
+      <c r="E448" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A449" s="1">
+        <v>44251</v>
+      </c>
+      <c r="E449" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A450" s="1">
+        <v>44252</v>
+      </c>
+      <c r="E450" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A451" s="1">
+        <v>44253</v>
+      </c>
+      <c r="E451" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A452" s="1">
+        <v>44254</v>
+      </c>
+      <c r="E452" s="4">
+        <f t="shared" ref="E452:E455" si="7">SUM(B452,C452,D452)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A453" s="1">
+        <v>44255</v>
+      </c>
+      <c r="E453" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E454" s="4"/>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E455" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hora de estudios de lunes 23 de feb del 2020
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D448" sqref="D448"/>
+      <selection pane="bottomLeft" activeCell="E447" sqref="E447:E453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7367,9 +7367,15 @@
       <c r="A448" s="1">
         <v>44250</v>
       </c>
+      <c r="B448" s="3">
+        <v>5.0138888888888893E-2</v>
+      </c>
+      <c r="D448" s="3">
+        <v>4.189814814814815E-2</v>
+      </c>
       <c r="E448" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>9.2037037037037042E-2</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -7404,7 +7410,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E455" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E453" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hora de estudios de lunes 25 de feb del 2020
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E447" sqref="E447:E453"/>
+      <selection pane="bottomLeft" activeCell="D451" sqref="D451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7382,18 +7382,36 @@
       <c r="A449" s="1">
         <v>44251</v>
       </c>
+      <c r="B449" s="3">
+        <v>4.4675925925925924E-2</v>
+      </c>
+      <c r="C449" s="3">
+        <v>4.9722222222222223E-2</v>
+      </c>
+      <c r="D449" s="3">
+        <v>2.9872685185185183E-2</v>
+      </c>
       <c r="E449" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.12427083333333333</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>44252</v>
       </c>
+      <c r="B450" s="3">
+        <v>3.875E-2</v>
+      </c>
+      <c r="C450" s="3">
+        <v>3.0740740740740739E-2</v>
+      </c>
+      <c r="D450" s="3">
+        <v>3.0439814814814819E-2</v>
+      </c>
       <c r="E450" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>9.9930555555555564E-2</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de lunes 26 de feb del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D451" sqref="D451"/>
+      <selection pane="bottomLeft" activeCell="D452" sqref="D452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7418,9 +7418,15 @@
       <c r="A451" s="1">
         <v>44253</v>
       </c>
+      <c r="B451" s="3">
+        <v>3.6805555555555557E-2</v>
+      </c>
+      <c r="D451" s="3">
+        <v>3.7928240740740742E-2</v>
+      </c>
       <c r="E451" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7.4733796296296298E-2</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de lunes 01 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2184,11 +2184,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O455"/>
+  <dimension ref="A1:O460"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D452" sqref="D452"/>
+      <selection pane="bottomLeft" activeCell="E454" sqref="E454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7434,7 +7434,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E453" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E460" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -7448,10 +7448,73 @@
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E454" s="4"/>
+      <c r="A454" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B454" s="3">
+        <v>4.0034722222222222E-2</v>
+      </c>
+      <c r="C454" s="3">
+        <v>3.681712962962963E-2</v>
+      </c>
+      <c r="E454" s="4">
+        <f t="shared" si="7"/>
+        <v>7.6851851851851852E-2</v>
+      </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E455" s="4"/>
+      <c r="A455" s="1">
+        <v>44257</v>
+      </c>
+      <c r="E455" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A456" s="1">
+        <v>44258</v>
+      </c>
+      <c r="E456" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A457" s="1">
+        <v>44259</v>
+      </c>
+      <c r="E457" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A458" s="1">
+        <v>44260</v>
+      </c>
+      <c r="E458" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A459" s="1">
+        <v>44261</v>
+      </c>
+      <c r="E459" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A460" s="1">
+        <v>44262</v>
+      </c>
+      <c r="E460" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hora de estudios de lunes 02 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E454" sqref="E454"/>
+      <selection pane="bottomLeft" activeCell="E454" sqref="E454:E460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7466,9 +7466,18 @@
       <c r="A455" s="1">
         <v>44257</v>
       </c>
+      <c r="B455" s="3">
+        <v>4.9513888888888892E-2</v>
+      </c>
+      <c r="C455" s="3">
+        <v>4.6273148148148147E-2</v>
+      </c>
+      <c r="D455" s="3">
+        <v>3.8680555555555558E-2</v>
+      </c>
       <c r="E455" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.13446759259259258</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de lunes 03 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E454" sqref="E454:E460"/>
+      <selection pane="bottomLeft" activeCell="D457" sqref="D457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7484,9 +7484,15 @@
       <c r="A456" s="1">
         <v>44258</v>
       </c>
+      <c r="B456" s="3">
+        <v>3.5277777777777776E-2</v>
+      </c>
+      <c r="D456" s="3">
+        <v>3.6273148148148145E-2</v>
+      </c>
       <c r="E456" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7.1550925925925921E-2</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de lunes 04 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D457" sqref="D457"/>
+      <selection pane="bottomLeft" activeCell="D458" sqref="D458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7499,9 +7499,18 @@
       <c r="A457" s="1">
         <v>44259</v>
       </c>
+      <c r="B457" s="3">
+        <v>4.2245370370370371E-2</v>
+      </c>
+      <c r="C457" s="3">
+        <v>3.9976851851851854E-2</v>
+      </c>
+      <c r="D457" s="3">
+        <v>3.1377314814814809E-2</v>
+      </c>
       <c r="E457" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.11359953703703704</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de lunes 05 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D458" sqref="D458"/>
+      <selection pane="bottomLeft" activeCell="D459" sqref="D459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7517,9 +7517,15 @@
       <c r="A458" s="1">
         <v>44260</v>
       </c>
+      <c r="B458" s="3">
+        <v>4.8275462962962958E-2</v>
+      </c>
+      <c r="D458" s="3">
+        <v>3.2881944444444443E-2</v>
+      </c>
       <c r="E458" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.11574074074074E-2</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de lunes 08 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2184,11 +2184,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O460"/>
+  <dimension ref="A1:O467"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D459" sqref="D459"/>
+      <pane ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E462" sqref="E462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7434,7 +7434,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E460" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E467" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -7542,6 +7542,75 @@
         <v>44262</v>
       </c>
       <c r="E460" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A461" s="1">
+        <v>44263</v>
+      </c>
+      <c r="B461" s="3">
+        <v>4.4525462962962968E-2</v>
+      </c>
+      <c r="D461" s="3">
+        <v>3.7870370370370367E-2</v>
+      </c>
+      <c r="E461" s="4">
+        <f t="shared" si="7"/>
+        <v>8.2395833333333335E-2</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A462" s="1">
+        <v>44264</v>
+      </c>
+      <c r="E462" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A463" s="1">
+        <v>44265</v>
+      </c>
+      <c r="E463" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A464" s="1">
+        <v>44266</v>
+      </c>
+      <c r="E464" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A465" s="1">
+        <v>44267</v>
+      </c>
+      <c r="E465" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A466" s="1">
+        <v>44268</v>
+      </c>
+      <c r="E466" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A467" s="1">
+        <v>44269</v>
+      </c>
+      <c r="E467" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios de Martes 09 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E462" sqref="E462"/>
+      <selection pane="bottomLeft" activeCell="D463" sqref="D463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7565,9 +7565,15 @@
       <c r="A462" s="1">
         <v>44264</v>
       </c>
+      <c r="B462" s="3">
+        <v>4.7118055555555559E-2</v>
+      </c>
+      <c r="D462" s="3">
+        <v>4.9340277777777775E-2</v>
+      </c>
       <c r="E462" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.645833333333334E-2</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de Miercoles 10 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D463" sqref="D463"/>
+      <selection pane="bottomLeft" activeCell="D464" sqref="D464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7580,9 +7580,15 @@
       <c r="A463" s="1">
         <v>44265</v>
       </c>
+      <c r="B463" s="3">
+        <v>5.1817129629629623E-2</v>
+      </c>
+      <c r="D463" s="3">
+        <v>3.7187499999999998E-2</v>
+      </c>
       <c r="E463" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.9004629629629628E-2</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios de Viernes 12 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2184,11 +2184,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O467"/>
+  <dimension ref="A1:O469"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D464" sqref="D464"/>
+      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B467" sqref="B467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7595,36 +7595,68 @@
       <c r="A464" s="1">
         <v>44266</v>
       </c>
+      <c r="B464" s="3">
+        <v>4.8194444444444449E-2</v>
+      </c>
+      <c r="C464" s="3">
+        <v>5.2719907407407403E-2</v>
+      </c>
+      <c r="D464" s="3">
+        <v>8.9085648148148136E-2</v>
+      </c>
       <c r="E464" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>44267</v>
       </c>
+      <c r="B465" s="3">
+        <v>4.3287037037037041E-2</v>
+      </c>
+      <c r="D465" s="3">
+        <v>5.9791666666666667E-2</v>
+      </c>
       <c r="E465" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.1030787037037037</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>44268</v>
       </c>
+      <c r="B466" s="3">
+        <v>4.3020833333333335E-2</v>
+      </c>
       <c r="E466" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.3020833333333335E-2</v>
+      </c>
+    </row>
+    <row r="467" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>44269</v>
       </c>
       <c r="E467" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
+      </c>
+      <c r="I467" s="3">
+        <v>4.1076388888888891E-2</v>
+      </c>
+    </row>
+    <row r="468" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I468" s="3">
+        <v>4.8009259259259258E-2</v>
+      </c>
+    </row>
+    <row r="469" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I469" s="4">
+        <f>SUM(I467:I468)</f>
+        <v>8.908564814814815E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hora de estudios de Martes 16 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2184,11 +2184,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O469"/>
+  <dimension ref="A1:O474"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B467" sqref="B467"/>
+      <selection pane="bottomLeft" activeCell="I467" sqref="I467:I470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7644,19 +7644,46 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I467" s="3">
-        <v>4.1076388888888891E-2</v>
-      </c>
+      <c r="I467" s="3"/>
     </row>
     <row r="468" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I468" s="3">
-        <v>4.8009259259259258E-2</v>
-      </c>
+      <c r="A468" s="1">
+        <v>44270</v>
+      </c>
+      <c r="I468" s="3"/>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I469" s="4">
-        <f>SUM(I467:I468)</f>
-        <v>8.908564814814815E-2</v>
+      <c r="A469" s="1">
+        <v>44271</v>
+      </c>
+      <c r="B469" s="3">
+        <v>3.8645833333333331E-2</v>
+      </c>
+      <c r="I469" s="4"/>
+    </row>
+    <row r="470" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A470" s="1">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="471" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A471" s="1">
+        <v>44273</v>
+      </c>
+    </row>
+    <row r="472" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A472" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="473" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A473" s="1">
+        <v>44275</v>
+      </c>
+    </row>
+    <row r="474" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A474" s="1">
+        <v>44276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
horas de estudio y preguntas de examen
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,13 +2188,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I467" sqref="I467:I470"/>
+      <selection pane="bottomLeft" activeCell="E467" sqref="E467:E474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7434,7 +7435,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E467" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E474" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -7650,6 +7651,10 @@
       <c r="A468" s="1">
         <v>44270</v>
       </c>
+      <c r="E468" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="I468" s="3"/>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.25">
@@ -7659,31 +7664,73 @@
       <c r="B469" s="3">
         <v>3.8645833333333331E-2</v>
       </c>
+      <c r="D469" s="3">
+        <v>6.548611111111112E-2</v>
+      </c>
+      <c r="E469" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10413194444444446</v>
+      </c>
       <c r="I469" s="4"/>
     </row>
     <row r="470" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>44272</v>
       </c>
+      <c r="B470" s="3">
+        <v>6.8159722222222219E-2</v>
+      </c>
+      <c r="D470" s="3">
+        <v>5.1377314814814813E-2</v>
+      </c>
+      <c r="E470" s="4">
+        <f t="shared" si="7"/>
+        <v>0.11953703703703702</v>
+      </c>
     </row>
     <row r="471" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>44273</v>
       </c>
+      <c r="B471" s="3">
+        <v>5.5011574074074067E-2</v>
+      </c>
+      <c r="D471" s="3">
+        <v>4.1180555555555554E-2</v>
+      </c>
+      <c r="E471" s="4">
+        <f t="shared" si="7"/>
+        <v>9.6192129629629614E-2</v>
+      </c>
     </row>
     <row r="472" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>44274</v>
       </c>
+      <c r="B472" s="3">
+        <v>4.2581018518518525E-2</v>
+      </c>
+      <c r="E472" s="4">
+        <f t="shared" si="7"/>
+        <v>4.2581018518518525E-2</v>
+      </c>
     </row>
     <row r="473" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <v>44275</v>
       </c>
+      <c r="E473" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="474" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>44276</v>
+      </c>
+      <c r="E474" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hora de estudios de Lunes 29 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2184,11 +2184,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O474"/>
+  <dimension ref="A1:O485"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E467" sqref="E467:E474"/>
+      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7435,7 +7435,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E474" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E485" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -7729,6 +7729,117 @@
         <v>44276</v>
       </c>
       <c r="E474" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A475" s="1">
+        <v>44277</v>
+      </c>
+      <c r="B475" s="3">
+        <v>5.0983796296296291E-2</v>
+      </c>
+      <c r="D475" s="3">
+        <v>4.9421296296296297E-2</v>
+      </c>
+      <c r="E475" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10040509259259259</v>
+      </c>
+    </row>
+    <row r="476" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A476" s="1">
+        <v>44278</v>
+      </c>
+      <c r="B476" s="3">
+        <v>4.6805555555555552E-2</v>
+      </c>
+      <c r="E476" s="4">
+        <f t="shared" si="7"/>
+        <v>4.6805555555555552E-2</v>
+      </c>
+    </row>
+    <row r="477" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A477" s="1">
+        <v>44279</v>
+      </c>
+      <c r="E477" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A478" s="1">
+        <v>44280</v>
+      </c>
+      <c r="E478" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A479" s="1">
+        <v>44281</v>
+      </c>
+      <c r="E479" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A480" s="1">
+        <v>44282</v>
+      </c>
+      <c r="E480" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A481" s="1">
+        <v>44283</v>
+      </c>
+      <c r="E481" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A482" s="1">
+        <v>44284</v>
+      </c>
+      <c r="B482" s="3">
+        <v>4.8171296296296295E-2</v>
+      </c>
+      <c r="E482" s="4">
+        <f t="shared" si="7"/>
+        <v>4.8171296296296295E-2</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A483" s="1">
+        <v>44285</v>
+      </c>
+      <c r="E483" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A484" s="1">
+        <v>44286</v>
+      </c>
+      <c r="E484" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A485" s="1">
+        <v>44287</v>
+      </c>
+      <c r="E485" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios de Lunes 30 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E485"/>
+      <selection pane="bottomLeft" activeCell="D484" sqref="D484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7812,18 +7812,27 @@
       <c r="B482" s="3">
         <v>4.8171296296296295E-2</v>
       </c>
+      <c r="D482" s="3">
+        <v>7.0555555555555552E-2</v>
+      </c>
       <c r="E482" s="4">
         <f t="shared" si="7"/>
-        <v>4.8171296296296295E-2</v>
+        <v>0.11872685185185185</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A483" s="1">
         <v>44285</v>
       </c>
+      <c r="B483" s="3">
+        <v>5.1956018518518519E-2</v>
+      </c>
+      <c r="D483" s="3">
+        <v>5.6365740740740744E-2</v>
+      </c>
       <c r="E483" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.10832175925925927</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 31 de Marzo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>dia</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      </t>
   </si>
 </sst>
 </file>
@@ -2187,8 +2190,8 @@
   <dimension ref="A1:O485"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D484" sqref="D484"/>
+      <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D492" sqref="D492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7839,14 +7842,23 @@
       <c r="A484" s="1">
         <v>44286</v>
       </c>
+      <c r="B484" s="3">
+        <v>4.9814814814814812E-2</v>
+      </c>
+      <c r="D484" s="3">
+        <v>4.5844907407407404E-2</v>
+      </c>
       <c r="E484" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.5659722222222215E-2</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A485" s="1">
         <v>44287</v>
+      </c>
+      <c r="D485" t="s">
+        <v>8</v>
       </c>
       <c r="E485" s="4">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
hora de estudios del 01 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O485"/>
+  <dimension ref="A1:O494"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D492" sqref="D492"/>
+      <selection pane="bottomLeft" activeCell="E488" sqref="E488:E494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7438,7 +7438,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E485" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E494" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -7861,6 +7861,96 @@
         <v>8</v>
       </c>
       <c r="E485" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A486" s="1">
+        <v>44288</v>
+      </c>
+      <c r="E486" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A487" s="1">
+        <v>44289</v>
+      </c>
+      <c r="E487" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A488" s="1">
+        <v>44290</v>
+      </c>
+      <c r="E488" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A489" s="1">
+        <v>44291</v>
+      </c>
+      <c r="B489" s="3">
+        <v>3.5983796296296298E-2</v>
+      </c>
+      <c r="C489" s="3">
+        <v>4.4236111111111115E-2</v>
+      </c>
+      <c r="D489" s="3">
+        <v>5.5150462962962964E-2</v>
+      </c>
+      <c r="E489" s="4">
+        <f t="shared" si="7"/>
+        <v>0.13537037037037039</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A490" s="1">
+        <v>44292</v>
+      </c>
+      <c r="E490" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A491" s="1">
+        <v>44293</v>
+      </c>
+      <c r="E491" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A492" s="1">
+        <v>44294</v>
+      </c>
+      <c r="E492" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A493" s="1">
+        <v>44295</v>
+      </c>
+      <c r="E493" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A494" s="1">
+        <v>44296</v>
+      </c>
+      <c r="E494" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios del 06 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2191,7 +2191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E488" sqref="E488:E494"/>
+      <selection pane="bottomLeft" activeCell="D491" sqref="D491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7914,9 +7914,15 @@
       <c r="A490" s="1">
         <v>44292</v>
       </c>
+      <c r="B490" s="3">
+        <v>5.063657407407407E-2</v>
+      </c>
+      <c r="D490" s="3">
+        <v>5.5347222222222221E-2</v>
+      </c>
       <c r="E490" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.10598379629629628</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 08 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2190,8 +2190,8 @@
   <dimension ref="A1:O494"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D491" sqref="D491"/>
+      <pane ySplit="1" topLeftCell="A479" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D493" sqref="D493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7929,18 +7929,30 @@
       <c r="A491" s="1">
         <v>44293</v>
       </c>
+      <c r="B491" s="3">
+        <v>2.6400462962962962E-2</v>
+      </c>
+      <c r="D491" s="3">
+        <v>4.3784722222222218E-2</v>
+      </c>
       <c r="E491" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7.0185185185185184E-2</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <v>44294</v>
       </c>
+      <c r="B492" s="3">
+        <v>4.6782407407407411E-2</v>
+      </c>
+      <c r="D492" s="3">
+        <v>4.9699074074074069E-2</v>
+      </c>
       <c r="E492" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.6481481481481474E-2</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 09 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2190,8 +2190,8 @@
   <dimension ref="A1:O494"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A479" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D493" sqref="D493"/>
+      <pane ySplit="1" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7959,9 +7959,12 @@
       <c r="A493" s="1">
         <v>44295</v>
       </c>
+      <c r="B493" s="3">
+        <v>4.65625E-2</v>
+      </c>
       <c r="E493" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.65625E-2</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 12 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O494"/>
+  <dimension ref="A1:O500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E494"/>
+      <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E492" sqref="E492:E500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7438,7 +7438,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E494" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E500" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -7972,6 +7972,66 @@
         <v>44296</v>
       </c>
       <c r="E494" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A495" s="1">
+        <v>44297</v>
+      </c>
+      <c r="E495" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A496" s="1">
+        <v>44298</v>
+      </c>
+      <c r="B496" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="D496" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="E496" s="4">
+        <f t="shared" si="7"/>
+        <v>9.0277777777777776E-2</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A497" s="1">
+        <v>44299</v>
+      </c>
+      <c r="E497" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A498" s="1">
+        <v>44300</v>
+      </c>
+      <c r="E498" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A499" s="1">
+        <v>44301</v>
+      </c>
+      <c r="E499" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A500" s="1">
+        <v>44302</v>
+      </c>
+      <c r="E500" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios del 13 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2191,7 +2191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E492" sqref="E492:E500"/>
+      <selection pane="bottomLeft" activeCell="E496" sqref="E496:E500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8004,9 +8004,15 @@
       <c r="A497" s="1">
         <v>44299</v>
       </c>
+      <c r="B497" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="D497" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
       <c r="E497" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.0277777777777776E-2</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 14 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2191,7 +2191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E496" sqref="E496:E500"/>
+      <selection pane="bottomLeft" activeCell="D498" sqref="D498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8019,9 +8019,15 @@
       <c r="A498" s="1">
         <v>44300</v>
       </c>
+      <c r="B498" s="3">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="D498" s="3">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="E498" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.7222222222222224E-2</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 15 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2191,7 +2191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D498" sqref="D498"/>
+      <selection pane="bottomLeft" activeCell="D499" sqref="D499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8034,9 +8034,15 @@
       <c r="A499" s="1">
         <v>44301</v>
       </c>
+      <c r="B499" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="D499" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
       <c r="E499" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.0277777777777776E-2</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 16 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2191,7 +2191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D499" sqref="D499"/>
+      <selection pane="bottomLeft" activeCell="D500" sqref="D500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8049,9 +8049,15 @@
       <c r="A500" s="1">
         <v>44302</v>
       </c>
+      <c r="B500" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D500" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E500" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hora de estudios del 19 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O500"/>
+  <dimension ref="A1:O509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D500" sqref="D500"/>
+      <selection pane="bottomLeft" activeCell="E503" sqref="E503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7438,7 +7438,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E500" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E509" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -8058,6 +8058,93 @@
       <c r="E500" s="4">
         <f t="shared" si="7"/>
         <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A501" s="1">
+        <v>44303</v>
+      </c>
+      <c r="E501" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A502" s="1">
+        <v>44304</v>
+      </c>
+      <c r="E502" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A503" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B503" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="D503" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="E503" s="4">
+        <f t="shared" si="7"/>
+        <v>9.0277777777777776E-2</v>
+      </c>
+    </row>
+    <row r="504" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A504" s="1">
+        <v>44306</v>
+      </c>
+      <c r="E504" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A505" s="1">
+        <v>44307</v>
+      </c>
+      <c r="E505" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="506" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A506" s="1">
+        <v>44308</v>
+      </c>
+      <c r="E506" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A507" s="1">
+        <v>44309</v>
+      </c>
+      <c r="E507" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A508" s="1">
+        <v>44310</v>
+      </c>
+      <c r="E508" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="509" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A509" s="1">
+        <v>44311</v>
+      </c>
+      <c r="E509" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hora de estudios del 20 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2191,7 +2191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E503" sqref="E503"/>
+      <selection pane="bottomLeft" activeCell="D504" sqref="D504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8097,9 +8097,15 @@
       <c r="A504" s="1">
         <v>44306</v>
       </c>
+      <c r="B504" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="D504" s="3">
+        <v>4.5138888888888888E-2</v>
+      </c>
       <c r="E504" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.0277777777777776E-2</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 21, 22, 23 Y 26 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O509"/>
+  <dimension ref="A1:O514"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D504" sqref="D504"/>
+      <pane ySplit="1" topLeftCell="A482" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E503" sqref="E503:E514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7438,7 +7438,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E509" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E514" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -8112,27 +8112,45 @@
       <c r="A505" s="1">
         <v>44307</v>
       </c>
+      <c r="B505" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D505" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E505" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A506" s="1">
         <v>44308</v>
       </c>
+      <c r="B506" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D506" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E506" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A507" s="1">
         <v>44309</v>
       </c>
+      <c r="B507" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D507" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E507" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -8149,6 +8167,54 @@
         <v>44311</v>
       </c>
       <c r="E509" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A510" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B510" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E510" s="4">
+        <f t="shared" si="7"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="511" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A511" s="1">
+        <v>44313</v>
+      </c>
+      <c r="E511" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A512" s="1">
+        <v>44314</v>
+      </c>
+      <c r="E512" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A513" s="1">
+        <v>44315</v>
+      </c>
+      <c r="E513" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A514" s="1">
+        <v>44316</v>
+      </c>
+      <c r="E514" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios del 27 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2190,8 +2190,8 @@
   <dimension ref="A1:O514"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A482" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E503" sqref="E503:E514"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8187,9 +8187,15 @@
       <c r="A511" s="1">
         <v>44313</v>
       </c>
+      <c r="B511" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D511" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E511" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 28 y 29 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2190,8 +2190,8 @@
   <dimension ref="A1:O514"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
+      <pane ySplit="1" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B513" sqref="B513:D513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8202,18 +8202,30 @@
       <c r="A512" s="1">
         <v>44314</v>
       </c>
+      <c r="B512" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D512" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E512" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A513" s="1">
         <v>44315</v>
       </c>
+      <c r="B513" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D513" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E513" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 30 de Abril del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O514"/>
+  <dimension ref="A1:O523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B513" sqref="B513:D513"/>
+      <selection pane="bottomLeft" activeCell="E514" sqref="E514:E523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7438,7 +7438,7 @@
         <v>44254</v>
       </c>
       <c r="E452" s="4">
-        <f t="shared" ref="E452:E514" si="7">SUM(B452,C452,D452)</f>
+        <f t="shared" ref="E452:E515" si="7">SUM(B452,C452,D452)</f>
         <v>0</v>
       </c>
     </row>
@@ -8220,20 +8220,111 @@
       <c r="B513" s="3">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D513" s="3">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="D513" s="3"/>
       <c r="E513" s="4">
         <f t="shared" si="7"/>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514" s="1">
         <v>44316</v>
       </c>
+      <c r="B514" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D514" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E514" s="4">
         <f t="shared" si="7"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A515" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B515" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D515" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E515" s="4">
+        <f t="shared" si="7"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A516" s="1">
+        <v>44318</v>
+      </c>
+      <c r="E516" s="4">
+        <f t="shared" ref="E516:E523" si="8">SUM(B516,C516,D516)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A517" s="1">
+        <v>44319</v>
+      </c>
+      <c r="E517" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A518" s="1">
+        <v>44320</v>
+      </c>
+      <c r="E518" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A519" s="1">
+        <v>44321</v>
+      </c>
+      <c r="E519" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A520" s="1">
+        <v>44322</v>
+      </c>
+      <c r="E520" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A521" s="1">
+        <v>44323</v>
+      </c>
+      <c r="E521" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A522" s="1">
+        <v>44324</v>
+      </c>
+      <c r="E522" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A523" s="1">
+        <v>44325</v>
+      </c>
+      <c r="E523" s="4">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hora de estudios del 6 de Mayo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2191,7 +2191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E514" sqref="E514:E523"/>
+      <selection pane="bottomLeft" activeCell="D520" sqref="D520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8269,36 +8269,60 @@
       <c r="A517" s="1">
         <v>44319</v>
       </c>
+      <c r="B517" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D517" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E517" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A518" s="1">
         <v>44320</v>
       </c>
+      <c r="B518" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D518" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E518" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519" s="1">
         <v>44321</v>
       </c>
+      <c r="B519" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D519" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E519" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520" s="1">
         <v>44322</v>
       </c>
+      <c r="B520" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D520" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E520" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 10 de Mayo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O523"/>
+  <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D520" sqref="D520"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8261,7 +8261,7 @@
         <v>44318</v>
       </c>
       <c r="E516" s="4">
-        <f t="shared" ref="E516:E523" si="8">SUM(B516,C516,D516)</f>
+        <f t="shared" ref="E516:E532" si="8">SUM(B516,C516,D516)</f>
         <v>0</v>
       </c>
     </row>
@@ -8329,9 +8329,15 @@
       <c r="A521" s="1">
         <v>44323</v>
       </c>
+      <c r="B521" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D521" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E521" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.25">
@@ -8348,6 +8354,93 @@
         <v>44325</v>
       </c>
       <c r="E523" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A524" s="1">
+        <v>44326</v>
+      </c>
+      <c r="B524" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D524" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E524" s="4">
+        <f t="shared" si="8"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A525" s="1">
+        <v>44327</v>
+      </c>
+      <c r="E525" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A526" s="1">
+        <v>44328</v>
+      </c>
+      <c r="E526" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A527" s="1">
+        <v>44329</v>
+      </c>
+      <c r="E527" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A528" s="1">
+        <v>44330</v>
+      </c>
+      <c r="E528" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A529" s="1">
+        <v>44331</v>
+      </c>
+      <c r="E529" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A530" s="1">
+        <v>44332</v>
+      </c>
+      <c r="E530" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A531" s="1">
+        <v>44333</v>
+      </c>
+      <c r="E531" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="532" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A532" s="1">
+        <v>44334</v>
+      </c>
+      <c r="E532" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios del 14 de Mayo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2190,8 +2190,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D528" sqref="D528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8377,36 +8377,57 @@
       <c r="A525" s="1">
         <v>44327</v>
       </c>
+      <c r="B525" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E525" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A526" s="1">
         <v>44328</v>
       </c>
+      <c r="B526" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D526" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E526" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A527" s="1">
         <v>44329</v>
       </c>
+      <c r="B527" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D527" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E527" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A528" s="1">
         <v>44330</v>
       </c>
+      <c r="B528" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D528" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E528" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 17 de Mayo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O532"/>
+  <dimension ref="A1:O537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D528" sqref="D528"/>
+      <selection pane="bottomLeft" activeCell="E528" sqref="E528:E537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8261,7 +8261,7 @@
         <v>44318</v>
       </c>
       <c r="E516" s="4">
-        <f t="shared" ref="E516:E532" si="8">SUM(B516,C516,D516)</f>
+        <f t="shared" ref="E516:E537" si="8">SUM(B516,C516,D516)</f>
         <v>0</v>
       </c>
     </row>
@@ -8452,9 +8452,15 @@
       <c r="A531" s="1">
         <v>44333</v>
       </c>
+      <c r="B531" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D531" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E531" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.25">
@@ -8462,6 +8468,51 @@
         <v>44334</v>
       </c>
       <c r="E532" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="533" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A533" s="1">
+        <v>44335</v>
+      </c>
+      <c r="E533" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A534" s="1">
+        <v>44336</v>
+      </c>
+      <c r="E534" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A535" s="1">
+        <v>44337</v>
+      </c>
+      <c r="E535" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A536" s="1">
+        <v>44338</v>
+      </c>
+      <c r="E536" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A537" s="1">
+        <v>44339</v>
+      </c>
+      <c r="E537" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios del 18 de Mayo del 2021 al 21 de mayo 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2190,8 +2190,8 @@
   <dimension ref="A1:O537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E528" sqref="E528:E537"/>
+      <pane ySplit="1" topLeftCell="A502" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8467,36 +8467,60 @@
       <c r="A532" s="1">
         <v>44334</v>
       </c>
+      <c r="B532" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D532" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E532" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A533" s="1">
         <v>44335</v>
       </c>
+      <c r="B533" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D533" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E533" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A534" s="1">
         <v>44336</v>
       </c>
+      <c r="B534" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D534" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E534" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A535" s="1">
         <v>44337</v>
       </c>
+      <c r="B535" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D535" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E535" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se agrega al al archivo de credenciales comando para ver el log en tiempo real tail hora de estudios del 24 de Mayo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -389,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O537"/>
+  <dimension ref="A1:O544"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A502" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E537"/>
+      <pane ySplit="1" topLeftCell="A530" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E419" sqref="E419:E544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8261,7 +8261,7 @@
         <v>44318</v>
       </c>
       <c r="E516" s="4">
-        <f t="shared" ref="E516:E537" si="8">SUM(B516,C516,D516)</f>
+        <f t="shared" ref="E516:E544" si="8">SUM(B516,C516,D516)</f>
         <v>0</v>
       </c>
     </row>
@@ -8537,6 +8537,75 @@
         <v>44339</v>
       </c>
       <c r="E537" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A538" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B538" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D538" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E538" s="4">
+        <f t="shared" si="8"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A539" s="1">
+        <v>44341</v>
+      </c>
+      <c r="E539" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A540" s="1">
+        <v>44342</v>
+      </c>
+      <c r="E540" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A541" s="1">
+        <v>44343</v>
+      </c>
+      <c r="E541" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A542" s="1">
+        <v>44344</v>
+      </c>
+      <c r="E542" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="543" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A543" s="1">
+        <v>44345</v>
+      </c>
+      <c r="E543" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A544" s="1">
+        <v>44346</v>
+      </c>
+      <c r="E544" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios del 24 de Mayo del 2021 al 28 de mayo 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2190,8 +2190,8 @@
   <dimension ref="A1:O544"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A530" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E419" sqref="E419:E544"/>
+      <pane ySplit="1" topLeftCell="A508" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D542" sqref="D542"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8560,36 +8560,60 @@
       <c r="A539" s="1">
         <v>44341</v>
       </c>
+      <c r="B539" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D539" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E539" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A540" s="1">
         <v>44342</v>
       </c>
+      <c r="B540" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D540" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E540" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A541" s="1">
         <v>44343</v>
       </c>
+      <c r="B541" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D541" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E541" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A542" s="1">
         <v>44344</v>
       </c>
+      <c r="B542" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D542" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E542" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hora de estudios del 31 de Mayo del 2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O544"/>
+  <dimension ref="A1:O551"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A508" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D542" sqref="D542"/>
+      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E542" sqref="E542:E551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8261,7 +8261,7 @@
         <v>44318</v>
       </c>
       <c r="E516" s="4">
-        <f t="shared" ref="E516:E544" si="8">SUM(B516,C516,D516)</f>
+        <f t="shared" ref="E516:E551" si="8">SUM(B516,C516,D516)</f>
         <v>0</v>
       </c>
     </row>
@@ -8630,6 +8630,75 @@
         <v>44346</v>
       </c>
       <c r="E544" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="545" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A545" s="1">
+        <v>44347</v>
+      </c>
+      <c r="B545" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D545" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E545" s="4">
+        <f t="shared" si="8"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A546" s="1">
+        <v>44348</v>
+      </c>
+      <c r="E546" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A547" s="1">
+        <v>44349</v>
+      </c>
+      <c r="E547" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A548" s="1">
+        <v>44350</v>
+      </c>
+      <c r="E548" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A549" s="1">
+        <v>44351</v>
+      </c>
+      <c r="E549" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A550" s="1">
+        <v>44352</v>
+      </c>
+      <c r="E550" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A551" s="1">
+        <v>44353</v>
+      </c>
+      <c r="E551" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
hora de estudios hasta 07-06-2021
</commit_message>
<xml_diff>
--- a/Horas invertidad de estudio.xlsx
+++ b/Horas invertidad de estudio.xlsx
@@ -2187,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O551"/>
+  <dimension ref="A1:O558"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E542" sqref="E542:E551"/>
+      <pane ySplit="1" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E545" sqref="E545:E558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8261,7 +8261,7 @@
         <v>44318</v>
       </c>
       <c r="E516" s="4">
-        <f t="shared" ref="E516:E551" si="8">SUM(B516,C516,D516)</f>
+        <f t="shared" ref="E516:E558" si="8">SUM(B516,C516,D516)</f>
         <v>0</v>
       </c>
     </row>
@@ -8653,36 +8653,60 @@
       <c r="A546" s="1">
         <v>44348</v>
       </c>
+      <c r="B546" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D546" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E546" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A547" s="1">
         <v>44349</v>
       </c>
+      <c r="B547" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D547" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E547" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A548" s="1">
         <v>44350</v>
       </c>
+      <c r="B548" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D548" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E548" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A549" s="1">
         <v>44351</v>
       </c>
+      <c r="B549" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D549" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E549" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
@@ -8699,6 +8723,75 @@
         <v>44353</v>
       </c>
       <c r="E551" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A552" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B552" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D552" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E552" s="4">
+        <f t="shared" si="8"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A553" s="1">
+        <v>44355</v>
+      </c>
+      <c r="E553" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A554" s="1">
+        <v>44356</v>
+      </c>
+      <c r="E554" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A555" s="1">
+        <v>44357</v>
+      </c>
+      <c r="E555" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A556" s="1">
+        <v>44358</v>
+      </c>
+      <c r="E556" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A557" s="1">
+        <v>44359</v>
+      </c>
+      <c r="E557" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A558" s="1">
+        <v>44360</v>
+      </c>
+      <c r="E558" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>

</xml_diff>